<commit_message>
Adjusted entries on fullspatialerrors_template
Cleaned up ruleDataItems
</commit_message>
<xml_diff>
--- a/fullspatialerrors_template.xlsx
+++ b/fullspatialerrors_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e122438\Documents\GitHub\hpms-validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE00325-6798-410F-ADFF-48E3A4BB4354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54998E6D-0780-4A8D-942D-A214CC277811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{97E3FA51-E252-4476-B25E-8BCEAF1F7C64}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{97E3FA51-E252-4476-B25E-8BCEAF1F7C64}"/>
   </bookViews>
   <sheets>
     <sheet name="ruleDataItems" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="513">
   <si>
     <t>Rule</t>
   </si>
@@ -1999,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2B6993-24F5-4E36-B923-10E570918712}">
   <dimension ref="A1:GA111"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2588,7 +2588,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>94</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>97</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>100</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>103</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>106</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>109</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>112</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>115</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>118</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>121</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>124</v>
       </c>
@@ -2771,13 +2771,13 @@
         <v>295</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>126</v>
       </c>
       <c r="B44" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>HPMS_SAMPLE_NO,CURVES_F,F_SYSTEM,URBAN_CODE,BMP,EMP</v>
+        <v>HPMS_SAMPLE_NO,CURVES_F</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>278</v>
@@ -2785,20 +2785,8 @@
       <c r="D44" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="E44" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>128</v>
       </c>
@@ -2819,7 +2807,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>131</v>
       </c>
@@ -2828,7 +2816,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>134</v>
       </c>
@@ -2852,31 +2840,19 @@
         <v>292</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>136</v>
       </c>
       <c r="B48" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>HPMS_SAMPLE_NO,F_SYSTEM,URBAN_CODE,GRADES_F,BMP,EMP</v>
+        <v>HPMS_SAMPLE_NO,GRADES_F</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>278</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="F48" s="5" t="s">
         <v>292</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -3470,7 +3446,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>218</v>
       </c>
@@ -3485,7 +3461,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>219</v>
       </c>
@@ -3500,7 +3476,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>221</v>
       </c>
@@ -3511,14 +3487,14 @@
       <c r="C83" s="5" t="s">
         <v>382</v>
       </c>
+      <c r="D83" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="E83" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="F83" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>224</v>
       </c>
@@ -3529,14 +3505,14 @@
       <c r="C84" s="5" t="s">
         <v>384</v>
       </c>
+      <c r="D84" s="5" t="s">
+        <v>385</v>
+      </c>
       <c r="E84" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="F84" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>226</v>
       </c>
@@ -3547,14 +3523,14 @@
       <c r="C85" s="5" t="s">
         <v>380</v>
       </c>
+      <c r="D85" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="E85" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="F85" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>227</v>
       </c>
@@ -3565,14 +3541,14 @@
       <c r="C86" s="5" t="s">
         <v>386</v>
       </c>
+      <c r="D86" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="E86" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="F86" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>229</v>
       </c>
@@ -3586,14 +3562,14 @@
       <c r="D87" s="5" t="s">
         <v>382</v>
       </c>
+      <c r="E87" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="F87" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G87" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>231</v>
       </c>
@@ -3607,14 +3583,14 @@
       <c r="D88" s="5" t="s">
         <v>384</v>
       </c>
+      <c r="E88" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="F88" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G88" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>232</v>
       </c>
@@ -3628,14 +3604,14 @@
       <c r="D89" s="5" t="s">
         <v>380</v>
       </c>
+      <c r="E89" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="F89" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G89" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>233</v>
       </c>
@@ -3649,14 +3625,14 @@
       <c r="D90" s="5" t="s">
         <v>386</v>
       </c>
+      <c r="E90" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="F90" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G90" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>234</v>
       </c>
@@ -3665,7 +3641,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>236</v>
       </c>
@@ -3674,7 +3650,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>238</v>
       </c>
@@ -3683,7 +3659,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>241</v>
       </c>
@@ -3695,7 +3671,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>243</v>
       </c>
@@ -3707,7 +3683,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>245</v>
       </c>

</xml_diff>

<commit_message>
Updated Logic to match FWHA checks
SJF43: Can't fix as curves values are being rounded
SJF47: Can't fix as grades values are being rounded
SJF49: Ignoring for now, only 3 values are different
SJF55: Ignoring for now, only 1 different
SJF64: FHWA logic is incorrect, flagging rows where Facility_type = 4 (should only check facility_type = 1,2,6)
SJF69: FHWA logic is incorrect, flagging rows where facility_type = 1,6 (should only check facility_type = 2)
</commit_message>
<xml_diff>
--- a/fullspatialerrors_template.xlsx
+++ b/fullspatialerrors_template.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e122438\Documents\GitHub\hpms-validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753D80E5-2A11-4275-9374-F20163507AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F813A0A7-7F77-4549-9DE6-3A1CD7B69E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{97E3FA51-E252-4476-B25E-8BCEAF1F7C64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{97E3FA51-E252-4476-B25E-8BCEAF1F7C64}"/>
   </bookViews>
   <sheets>
     <sheet name="ruleDataItems" sheetId="3" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Summary!$A$1:$G$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Summary!$A$1:$H$107</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="524">
   <si>
     <t>Rule</t>
   </si>
@@ -1579,6 +1579,39 @@
   </si>
   <si>
     <t>SJF100</t>
+  </si>
+  <si>
+    <t>FWHA Num Failed</t>
+  </si>
+  <si>
+    <t>CURVES_A</t>
+  </si>
+  <si>
+    <t>CURVES_B</t>
+  </si>
+  <si>
+    <t>CURVES_C</t>
+  </si>
+  <si>
+    <t>CURVES_D</t>
+  </si>
+  <si>
+    <t>CURVES_E</t>
+  </si>
+  <si>
+    <t>GRADES_A</t>
+  </si>
+  <si>
+    <t>GRADES_B</t>
+  </si>
+  <si>
+    <t>GRADES_C</t>
+  </si>
+  <si>
+    <t>GRADES_D</t>
+  </si>
+  <si>
+    <t>GRADES_E</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1644,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1625,7 +1657,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1648,12 +1680,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1670,9 +1713,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1997,10 +2046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2B6993-24F5-4E36-B923-10E570918712}">
-  <dimension ref="A1:GA111"/>
+  <dimension ref="A1:GK111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48:I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,10 +2077,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="str">
+      <c r="B2" s="6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,C2:AG2)</f>
         <v>FACILITY_TYPE,F_SYSTEM</v>
       </c>
@@ -2043,10 +2092,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="str">
+      <c r="B3" s="6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,C3:AG3)</f>
         <v>FACILITY_TYPE,F_SYSTEM,URBAN_CODE,DIR_THROUGH_LANES,IRI</v>
       </c>
@@ -2067,10 +2116,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="7" t="str">
+      <c r="B4" s="6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,C4:AG4)</f>
         <v>FACILITY_TYPE,F_SYSTEM</v>
       </c>
@@ -2082,19 +2131,19 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="7" t="str">
+      <c r="B5" s="6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,C5:AG5)</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="7" t="str">
+      <c r="B6" s="6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,C6:AG6)</f>
         <v>FACILITY_TYPE,F_SYSTEM,HPMS_SAMPLE_NO,NHS,ACCESS_CONTROL</v>
       </c>
@@ -2115,10 +2164,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="7" t="str">
+      <c r="B7" s="6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,C7:N7)</f>
         <v>FACILITY_TYPE,F_SYSTEM,OWNERSHIP</v>
       </c>
@@ -2133,10 +2182,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="7" t="str">
+      <c r="B8" s="6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,C8:N8)</f>
         <v>FACILITY_TYPE,F_SYSTEM,NHS,URBAN_CODE,THROUGH_LANES</v>
       </c>
@@ -2157,28 +2206,28 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="7" t="str">
+      <c r="B9" s="6" t="str">
         <f t="shared" ref="B9:B72" si="0">_xlfn.TEXTJOIN(",",TRUE,C9:N9)</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="7" t="str">
+      <c r="B10" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="7" t="str">
+      <c r="B11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,PEAK_LANES</v>
       </c>
@@ -2190,10 +2239,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="7" t="str">
+      <c r="B12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,FACILITY_TYPE,URBAN_CODE,THROUGH_LANES,COUNTER_PEAK_LANES</v>
       </c>
@@ -2214,10 +2263,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="7" t="str">
+      <c r="B13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,TURN_LANES_R,URBAN_CODE,ACCESS_CONTROL</v>
       </c>
@@ -2235,10 +2284,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="7" t="str">
+      <c r="B14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,TURN_LANES_L,URBAN_CODE,ACCESS_CONTROL</v>
       </c>
@@ -2256,10 +2305,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="7" t="str">
+      <c r="B15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,NHS,SPEED_LIMIT</v>
       </c>
@@ -2274,19 +2323,19 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="7" t="str">
+      <c r="B16" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="7" t="str">
+      <c r="B17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>F_SYSTEM,FACILITY_TYPE,ROUTE_SIGNING,ROUTE_NUMBER,DIR_THROUGH_LANES,IRI</v>
       </c>
@@ -2310,10 +2359,10 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="7" t="str">
+      <c r="B18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>F_SYSTEM,NHS,FACILITY_TYPE,ROUTE_SIGNING</v>
       </c>
@@ -2331,10 +2380,10 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="7" t="str">
+      <c r="B19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>F_SYSTEM,NHS,FACILITY_TYPE,ROUTE_QUALIFIER</v>
       </c>
@@ -2352,10 +2401,10 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="7" t="str">
+      <c r="B20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>F_SYSTEM,NHS,FACILITY_TYPE,ROUTE_NAME_VALUE_TEXT</v>
       </c>
@@ -2373,10 +2422,10 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="7" t="str">
+      <c r="B21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>FACILITY_TYPE,F_SYSTEM,URBAN_CODE,NHS,AADT</v>
       </c>
@@ -2397,10 +2446,10 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="7" t="str">
+      <c r="B22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,F_SYSTEM,FACILITY_TYPE,AADT_SINGLE_UNIT</v>
       </c>
@@ -2418,10 +2467,10 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="7" t="str">
+      <c r="B23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,PCT_DH_SINGLE_UNIT</v>
       </c>
@@ -2433,10 +2482,10 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="7" t="str">
+      <c r="B24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,F_SYSTEM,FACILITY_TYPE,AADT_COMBINATION</v>
       </c>
@@ -2454,10 +2503,10 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="7" t="str">
+      <c r="B25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,PCT_DH_COMBINATION</v>
       </c>
@@ -2469,10 +2518,10 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="7" t="str">
+      <c r="B26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,K_FACTOR</v>
       </c>
@@ -2484,10 +2533,10 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="7" t="str">
+      <c r="B27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,DIR_FACTOR</v>
       </c>
@@ -2499,10 +2548,10 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="7" t="str">
+      <c r="B28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,FUTURE_AADT</v>
       </c>
@@ -2514,10 +2563,10 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="7" t="str">
+      <c r="B29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>URBAN_CODE,NUMBER_SIGNALS,HPMS_SAMPLE_NO,SIGNAL_TYPE</v>
       </c>
@@ -2535,10 +2584,10 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="7" t="str">
+      <c r="B30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>URBAN_CODE,NUMBER_SIGNALS,HPMS_SAMPLE_NO,PCT_GREEN_TIME</v>
       </c>
@@ -2556,10 +2605,10 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="7" t="str">
+      <c r="B31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,NUMBER_SIGNALS,SIGNAL_TYPE</v>
       </c>
@@ -2574,10 +2623,10 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B32" s="7" t="str">
+      <c r="B32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,STOP_SIGNS</v>
       </c>
@@ -2588,11 +2637,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="7" t="str">
+      <c r="B33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,AT_GRADE_OTHER</v>
       </c>
@@ -2603,11 +2652,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="7" t="str">
+      <c r="B34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,LANE_WIDTH</v>
       </c>
@@ -2618,11 +2667,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B35" s="7" t="str">
+      <c r="B35" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,MEDIAN_TYPE</v>
       </c>
@@ -2633,11 +2682,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B36" s="7" t="str">
+      <c r="B36" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,MEDIAN_TYPE,MEDIAN_WIDTH</v>
       </c>
@@ -2651,11 +2700,11 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="7" t="str">
+      <c r="B37" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,SHOULDER_TYPE</v>
       </c>
@@ -2666,11 +2715,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="7" t="str">
+      <c r="B38" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,SHOULDER_TYPE,SHOULDER_WIDTH_R</v>
       </c>
@@ -2684,11 +2733,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="7" t="str">
+      <c r="B39" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,SHOULDER_TYPE,SHOULDER_WIDTH_L,MEDIAN_TYPE</v>
       </c>
@@ -2705,11 +2754,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B40" s="7" t="str">
+      <c r="B40" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,URBAN_CODE,PEAK_PARKING</v>
       </c>
@@ -2723,11 +2772,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B41" s="7" t="str">
+      <c r="B41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,WIDENING_POTENTIAL</v>
       </c>
@@ -2738,22 +2787,22 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="7" t="str">
+      <c r="B42" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B43" s="7" t="str">
+      <c r="B43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>HPMS_SAMPLE_NO,F_SYSTEM,URBAN_CODE,SURFACE_TYPE,CURVES_F</v>
+        <v>HPMS_SAMPLE_NO,F_SYSTEM,URBAN_CODE,SURFACE_TYPE,CURVES_A,CURVES_B,CURVES_C,CURVES_D,CURVES_E,CURVES_F</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>278</v>
@@ -2768,29 +2817,65 @@
         <v>148</v>
       </c>
       <c r="G43" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="L43" s="5" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="7" t="str">
+      <c r="B44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>HPMS_SAMPLE_NO,CURVES_F</v>
+        <v>HPMS_SAMPLE_NO,F_SYSTEM,URBAN_CODE,CURVES_A,CURVES_B,CURVES_C,CURVES_D,CURVES_E,CURVES_F</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>278</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="K44" s="5" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B45" s="7" t="str">
+      <c r="B45" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,URBAN_CODE,F_SYSTEM,TERRAIN_TYPE</v>
       </c>
@@ -2807,22 +2892,22 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B46" s="7" t="str">
+      <c r="B46" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="7" t="str">
+      <c r="B47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>HPMS_SAMPLE_NO,F_SYSTEM,URBAN_CODE,SURFACE_TYPE,GRADES_F</v>
+        <v>HPMS_SAMPLE_NO,F_SYSTEM,URBAN_CODE,SURFACE_TYPE,GRADES_A,GRADES_B,GRADES_C,GRADES_D,GRADES_E,GRADES_F</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>278</v>
@@ -2836,30 +2921,60 @@
       <c r="F47" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="G47" s="9" t="s">
+        <v>519</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="J47" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="L47" s="5" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B48" s="7" t="str">
+      <c r="B48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>HPMS_SAMPLE_NO,GRADES_F</v>
+        <v>HPMS_SAMPLE_NO,GRADES_A,GRADES_B,GRADES_C,GRADES_D,GRADES_E,GRADES_F</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="9" t="s">
+        <v>519</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="I48" s="5" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B49" s="7" t="str">
+      <c r="B49" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,URBAN_CODE,THROUGH_LANES,MEDIAN_TYPE,SURFACE_TYPE,PCT_PASS_SIGHT</v>
       </c>
@@ -2883,10 +2998,10 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="B50" s="7" t="str">
+      <c r="B50" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,SURFACE_TYPE,FACILITY_TYPE,F_SYSTEM,DIR_THROUGH_LANES,URBAN_CODE,IRI</v>
       </c>
@@ -2913,19 +3028,19 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B51" s="7" t="str">
+      <c r="B51" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B52" s="7" t="str">
+      <c r="B52" s="6" t="str">
         <f t="shared" si="0"/>
         <v>FACILITY_TYPE,F_SYSTEM,NHS,HPMS_SAMPLE_NO,DIR_THROUGH_LANES,IRI,SURFACE_TYPE</v>
       </c>
@@ -2952,10 +3067,10 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B53" s="7" t="str">
+      <c r="B53" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SURFACE_TYPE,FACILITY_TYPE,F_SYSTEM,NHS,HPMS_SAMPLE_NO,DIR_THROUGH_LANES,IRI,RUTTING</v>
       </c>
@@ -2985,10 +3100,10 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="B54" s="7" t="str">
+      <c r="B54" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SURFACE_TYPE,FACILITY_TYPE,F_SYSTEM,NHS,HPMS_SAMPLE_NO,DIR_THROUGH_LANES,IRI,FAULTING</v>
       </c>
@@ -3018,10 +3133,10 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B55" s="7" t="str">
+      <c r="B55" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SURFACE_TYPE,FACILITY_TYPE,F_SYSTEM,NHS,HPMS_SAMPLE_NO,DIR_THROUGH_LANES,IRI,CRACKING_PERCENT</v>
       </c>
@@ -3051,10 +3166,10 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B56" s="7" t="str">
+      <c r="B56" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,SURFACE_TYPE,YEAR_LAST_CONSTRUCTION_VALUE_DATE,YEAR_LAST_IMPROVEMENT_VALUE_DATE</v>
       </c>
@@ -3072,10 +3187,10 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B57" s="7" t="str">
+      <c r="B57" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,SURFACE_TYPE,YEAR_LAST_CONSTRUCTION_VALUE_DATE</v>
       </c>
@@ -3090,10 +3205,10 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B58" s="7" t="str">
+      <c r="B58" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,YEAR_LAST_IMPROVEMENT_VALUE_DATE,LAST_OVERLAY_THICKNESS</v>
       </c>
@@ -3108,10 +3223,10 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B59" s="7" t="str">
+      <c r="B59" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SURFACE_TYPE,HPMS_SAMPLE_NO,THICKNESS_RIGID</v>
       </c>
@@ -3126,10 +3241,10 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B60" s="7" t="str">
+      <c r="B60" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SURFACE_TYPE,HPMS_SAMPLE_NO,THICKNESS_FLEXIBLE</v>
       </c>
@@ -3144,10 +3259,10 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B61" s="7" t="str">
+      <c r="B61" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HPMS_SAMPLE_NO,SURFACE_TYPE,BASE_TYPE</v>
       </c>
@@ -3162,10 +3277,10 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B62" s="7" t="str">
+      <c r="B62" s="6" t="str">
         <f t="shared" si="0"/>
         <v>BASE_TYPE,SURFACE_TYPE,HPMS_SAMPLE_NO,BASE_THICKNESS</v>
       </c>
@@ -3183,19 +3298,19 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B63" s="7" t="str">
+      <c r="B63" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B64" s="7" t="str">
+      <c r="B64" s="6" t="str">
         <f t="shared" si="0"/>
         <v>FACILITY_TYPE,F_SYSTEM,URBAN_CODE,COUNTY_ID</v>
       </c>
@@ -3213,10 +3328,10 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
+      <c r="A65" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="B65" s="7" t="str">
+      <c r="B65" s="6" t="str">
         <f t="shared" si="0"/>
         <v>F_SYSTEM,FACILITY_TYPE,NHS</v>
       </c>
@@ -3231,37 +3346,37 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B66" s="7" t="str">
+      <c r="B66" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="B67" s="7" t="str">
+      <c r="B67" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="B68" s="7" t="str">
+      <c r="B68" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
+      <c r="A69" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="B69" s="7" t="str">
+      <c r="B69" s="6" t="str">
         <f t="shared" si="0"/>
         <v>F_SYSTEM,FACILITY_TYPE,IRI,DIR_THROUGH_LANES</v>
       </c>
@@ -3279,10 +3394,10 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="B70" s="7" t="str">
+      <c r="B70" s="6" t="str">
         <f t="shared" si="0"/>
         <v>FACILITY_TYPE,THROUGH_LANES</v>
       </c>
@@ -3294,10 +3409,10 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="B71" s="7" t="str">
+      <c r="B71" s="6" t="str">
         <f t="shared" si="0"/>
         <v>COUNTER_PEAK_LANES,PEAK_LANES,THROUGH_LANES</v>
       </c>
@@ -3312,10 +3427,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="B72" s="7" t="str">
+      <c r="B72" s="6" t="str">
         <f t="shared" si="0"/>
         <v>FACILITY_TYPE,COUNTER_PEAK_LANES</v>
       </c>
@@ -3327,10 +3442,10 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="B73" s="7" t="str">
+      <c r="B73" s="6" t="str">
         <f t="shared" ref="B73:B107" si="1">_xlfn.TEXTJOIN(",",TRUE,C73:N73)</f>
         <v>SPEED_LIMIT</v>
       </c>
@@ -3339,10 +3454,10 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="B74" s="7" t="str">
+      <c r="B74" s="6" t="str">
         <f t="shared" si="1"/>
         <v>F_SYSTEM,URBAN_CODE,SIGNAL_TYPE</v>
       </c>
@@ -3357,10 +3472,10 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="B75" s="7" t="str">
+      <c r="B75" s="6" t="str">
         <f t="shared" si="1"/>
         <v>LANE_WIDTH</v>
       </c>
@@ -3369,10 +3484,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="B76" s="7" t="str">
+      <c r="B76" s="6" t="str">
         <f t="shared" si="1"/>
         <v>MEDIAN_WIDTH,MEDIAN_TYPE</v>
       </c>
@@ -3384,10 +3499,10 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B77" s="7" t="str">
+      <c r="B77" s="6" t="str">
         <f t="shared" si="1"/>
         <v>FACILITY_TYPE,MEDIAN_TYPE,MEDIAN_WIDTH</v>
       </c>
@@ -3402,10 +3517,10 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="B78" s="7" t="str">
+      <c r="B78" s="6" t="str">
         <f t="shared" si="1"/>
         <v>MEDIAN_WIDTH,SHOULDER_WIDTH_L</v>
       </c>
@@ -3417,10 +3532,10 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="B79" s="7" t="str">
+      <c r="B79" s="6" t="str">
         <f t="shared" si="1"/>
         <v>IRI_VALUE_DATE,HPMS_SAMPLE_NO</v>
       </c>
@@ -3432,10 +3547,10 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="B80" s="7" t="str">
+      <c r="B80" s="6" t="str">
         <f t="shared" si="1"/>
         <v>RUTTING_VALUE_DATE,HPMS_SAMPLE_NO</v>
       </c>
@@ -3447,10 +3562,10 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B81" s="7" t="str">
+      <c r="B81" s="6" t="str">
         <f t="shared" si="1"/>
         <v>FAULTING_VALUE_DATE,HPMS_SAMPLE_NO</v>
       </c>
@@ -3462,10 +3577,10 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="B82" s="7" t="str">
+      <c r="B82" s="6" t="str">
         <f t="shared" si="1"/>
         <v>CRACKING_PERCENT_VALUE_DATE,HPMS_SAMPLE_NO</v>
       </c>
@@ -3477,10 +3592,10 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="B83" s="7" t="str">
+      <c r="B83" s="6" t="str">
         <f t="shared" si="1"/>
         <v>CRACKING_PERCENT_VALUE_DATE,CRACKING_PERCENT_VALUE_TEXT,F_SYSTEM</v>
       </c>
@@ -3495,10 +3610,10 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="B84" s="7" t="str">
+      <c r="B84" s="6" t="str">
         <f t="shared" si="1"/>
         <v>FAULTING_VALUE_DATE,FAULTING_VALUE_TEXT,F_SYSTEM</v>
       </c>
@@ -3513,10 +3628,10 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="B85" s="7" t="str">
+      <c r="B85" s="6" t="str">
         <f t="shared" si="1"/>
         <v>IRI_VALUE_DATE,IRI_VALUE_TEXT,F_SYSTEM</v>
       </c>
@@ -3531,10 +3646,10 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
+      <c r="A86" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="B86" s="7" t="str">
+      <c r="B86" s="6" t="str">
         <f t="shared" si="1"/>
         <v>RUTTING_VALUE_DATE,RUTTING_VALUE_TEXT,F_SYSTEM</v>
       </c>
@@ -3549,10 +3664,10 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
+      <c r="A87" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="B87" s="7" t="str">
+      <c r="B87" s="6" t="str">
         <f t="shared" si="1"/>
         <v>CRACKING_PERCENT_VALUE_TEXT,CRACKING_PERCENT_VALUE_DATE,F_SYSTEM,NHS</v>
       </c>
@@ -3570,10 +3685,10 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="B88" s="7" t="str">
+      <c r="B88" s="6" t="str">
         <f t="shared" si="1"/>
         <v>FAULTING_VALUE_TEXT,FAULTING_VALUE_DATE,F_SYSTEM,NHS</v>
       </c>
@@ -3591,10 +3706,10 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B89" s="7" t="str">
+      <c r="B89" s="6" t="str">
         <f t="shared" si="1"/>
         <v>IRI_VALUE_TEXT,IRI_VALUE_DATE,F_SYSTEM,NHS</v>
       </c>
@@ -3612,10 +3727,10 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="B90" s="7" t="str">
+      <c r="B90" s="6" t="str">
         <f t="shared" si="1"/>
         <v>RUTTING_VALUE_TEXT,RUTTING_VALUE_DATE,F_SYSTEM,NHS</v>
       </c>
@@ -3633,37 +3748,37 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="7" t="s">
+      <c r="A91" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B91" s="7" t="str">
+      <c r="B91" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B92" s="7" t="str">
+      <c r="B92" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="7" t="s">
+      <c r="A93" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="B93" s="7" t="str">
+      <c r="B93" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="B94" s="7" t="str">
+      <c r="B94" s="6" t="str">
         <f t="shared" si="1"/>
         <v>RUTTING</v>
       </c>
@@ -3672,10 +3787,10 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="7" t="s">
+      <c r="A95" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="B95" s="7" t="str">
+      <c r="B95" s="6" t="str">
         <f t="shared" si="1"/>
         <v>FAULTING</v>
       </c>
@@ -3684,10 +3799,10 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="7" t="s">
+      <c r="A96" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="B96" s="7" t="str">
+      <c r="B96" s="6" t="str">
         <f t="shared" si="1"/>
         <v>SURFACE_TYPE,LANE_WIDTH</v>
       </c>
@@ -3698,11 +3813,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="97" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="A97" s="7" t="s">
+    <row r="97" spans="1:193" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="B97" s="7" t="str">
+      <c r="B97" s="6" t="str">
         <f t="shared" si="1"/>
         <v>SURFACE_TYPE,CRACKING_PERCENT</v>
       </c>
@@ -3713,11 +3828,11 @@
         <v>157</v>
       </c>
     </row>
-    <row r="98" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
+    <row r="98" spans="1:193" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="B98" s="7" t="str">
+      <c r="B98" s="6" t="str">
         <f t="shared" si="1"/>
         <v>YEAR_LAST_CONSTRUCTION_VALUE_DATE</v>
       </c>
@@ -3725,11 +3840,11 @@
         <v>390</v>
       </c>
     </row>
-    <row r="99" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="A99" s="7" t="s">
+    <row r="99" spans="1:193" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B99" s="7" t="str">
+      <c r="B99" s="6" t="str">
         <f t="shared" si="1"/>
         <v>SURFACE_TYPE,THICKNESS_RIGID</v>
       </c>
@@ -3740,11 +3855,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="100" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="A100" s="7" t="s">
+    <row r="100" spans="1:193" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B100" s="7" t="str">
+      <c r="B100" s="6" t="str">
         <f t="shared" si="1"/>
         <v>SURFACE_TYPE,THICKNESS_FLEXIBLE</v>
       </c>
@@ -3755,11 +3870,11 @@
         <v>172</v>
       </c>
     </row>
-    <row r="101" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="A101" s="7" t="s">
+    <row r="101" spans="1:193" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="B101" s="7" t="str">
+      <c r="B101" s="6" t="str">
         <f t="shared" si="1"/>
         <v>SURFACE_TYPE,THICKNESS_FLEXIBLE</v>
       </c>
@@ -3770,11 +3885,11 @@
         <v>172</v>
       </c>
     </row>
-    <row r="102" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="A102" s="7" t="s">
+    <row r="102" spans="1:193" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="B102" s="7" t="str">
+      <c r="B102" s="6" t="str">
         <f t="shared" si="1"/>
         <v>SURFACE_TYPE,THICKNESS_RIGID</v>
       </c>
@@ -3785,11 +3900,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="103" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="A103" s="7" t="s">
+    <row r="103" spans="1:193" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="B103" s="7" t="str">
+      <c r="B103" s="6" t="str">
         <f t="shared" si="1"/>
         <v>DIR_THROUGH_LANES,THROUGH_LANES</v>
       </c>
@@ -3800,20 +3915,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="A104" s="7" t="s">
+    <row r="104" spans="1:193" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="B104" s="7" t="str">
+      <c r="B104" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="A105" s="7" t="s">
+    <row r="105" spans="1:193" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="B105" s="7" t="str">
+      <c r="B105" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OWNERSHIP,MAINTENANCE_OPERATIONS</v>
       </c>
@@ -3824,17 +3939,17 @@
         <v>193</v>
       </c>
     </row>
-    <row r="106" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="A106" s="7" t="s">
+    <row r="106" spans="1:193" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="B106" s="7"/>
-    </row>
-    <row r="107" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="A107" s="7" t="s">
+      <c r="B106" s="6"/>
+    </row>
+    <row r="107" spans="1:193" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="B107" s="7" t="str">
+      <c r="B107" s="6" t="str">
         <f t="shared" si="1"/>
         <v>FACILITY_TYPE,F_SYSTEM,URBAN_CODE,HPMS_SAMPLE_NO</v>
       </c>
@@ -3851,12 +3966,12 @@
         <v>278</v>
       </c>
     </row>
-    <row r="110" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:193" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="111" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:193" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>47</v>
       </c>
@@ -4406,10 +4521,40 @@
       <c r="GA111" t="s">
         <v>406</v>
       </c>
+      <c r="GB111" t="s">
+        <v>514</v>
+      </c>
+      <c r="GC111" t="s">
+        <v>515</v>
+      </c>
+      <c r="GD111" t="s">
+        <v>516</v>
+      </c>
+      <c r="GE111" t="s">
+        <v>517</v>
+      </c>
+      <c r="GF111" t="s">
+        <v>518</v>
+      </c>
+      <c r="GG111" t="s">
+        <v>519</v>
+      </c>
+      <c r="GH111" t="s">
+        <v>520</v>
+      </c>
+      <c r="GI111" t="s">
+        <v>521</v>
+      </c>
+      <c r="GJ111" t="s">
+        <v>522</v>
+      </c>
+      <c r="GK111" t="s">
+        <v>523</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C2:BL21 C22:F22 H22:BL22 U23:BL107 C23:T51" xr:uid="{83B01C7A-368D-4408-8F6C-876D6B156AF6}">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C2:BL21 C23:T43 C22:F22 F44:T44 U23:BL107 H22:BL22 L45:T51 G45:K46 J48:K51 C44:C51 D45:F47 D49:I51 I48" xr:uid="{83B01C7A-368D-4408-8F6C-876D6B156AF6}">
       <formula1>$111:$111</formula1>
     </dataValidation>
     <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C52:T107" xr:uid="{10AE5958-CEE7-4FF9-AC3E-2CBB6F4572BC}">
@@ -4422,9 +4567,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEACE931-9432-4CAA-874D-46D06D5BC6FB}">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B91" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4437,9 +4582,10 @@
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
     <col min="6" max="6" width="22.140625" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4461,8 +4607,11 @@
       <c r="G1" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="8" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>407</v>
       </c>
@@ -4477,7 +4626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>408</v>
       </c>
@@ -4491,9 +4640,9 @@
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>409</v>
       </c>
@@ -4508,7 +4657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>410</v>
       </c>
@@ -4523,7 +4672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>411</v>
       </c>
@@ -4538,7 +4687,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>412</v>
       </c>
@@ -4553,7 +4702,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>413</v>
       </c>
@@ -4568,7 +4717,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>414</v>
       </c>
@@ -4583,7 +4732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>415</v>
       </c>
@@ -4598,7 +4747,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>416</v>
       </c>
@@ -4613,7 +4762,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>417</v>
       </c>
@@ -4628,7 +4777,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>418</v>
       </c>
@@ -4643,7 +4792,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>419</v>
       </c>
@@ -4658,7 +4807,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>420</v>
       </c>
@@ -4673,7 +4822,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>421</v>
       </c>
@@ -6042,7 +6191,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G107" xr:uid="{BEACE931-9432-4CAA-874D-46D06D5BC6FB}"/>
+  <autoFilter ref="A1:H107" xr:uid="{BEACE931-9432-4CAA-874D-46D06D5BC6FB}"/>
   <conditionalFormatting sqref="B2:B108">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>ISREF(INDIRECT(A2&amp;"!A1"))</formula>

</xml_diff>

<commit_message>
Logic & template update
Added BEGIN_DATE column to DF if it does not exist after being loaded in. Removed all logic that used datetime.now() and replaced with tempDF['BEGIN_DATE']

Added BEGIN_DATE to data items in the template
</commit_message>
<xml_diff>
--- a/fullspatialerrors_template.xlsx
+++ b/fullspatialerrors_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e122438\Documents\GitHub\hpms-validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F813A0A7-7F77-4549-9DE6-3A1CD7B69E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1180171-930F-4078-BF74-7655D9876708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{97E3FA51-E252-4476-B25E-8BCEAF1F7C64}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{97E3FA51-E252-4476-B25E-8BCEAF1F7C64}"/>
   </bookViews>
   <sheets>
     <sheet name="ruleDataItems" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="525">
   <si>
     <t>Rule</t>
   </si>
@@ -1612,6 +1612,9 @@
   </si>
   <si>
     <t>GRADES_E</t>
+  </si>
+  <si>
+    <t>BEGIN_DATE</t>
   </si>
 </sst>
 </file>
@@ -2046,10 +2049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2B6993-24F5-4E36-B923-10E570918712}">
-  <dimension ref="A1:GK111"/>
+  <dimension ref="A1:GL111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48:I48"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3171,7 +3174,7 @@
       </c>
       <c r="B56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>HPMS_SAMPLE_NO,SURFACE_TYPE,YEAR_LAST_CONSTRUCTION_VALUE_DATE,YEAR_LAST_IMPROVEMENT_VALUE_DATE</v>
+        <v>HPMS_SAMPLE_NO,SURFACE_TYPE,YEAR_LAST_CONSTRUCTION_VALUE_DATE,YEAR_LAST_IMPROVEMENT_VALUE_DATE,BEGIN_DATE</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>278</v>
@@ -3184,6 +3187,9 @@
       </c>
       <c r="F56" s="5" t="s">
         <v>398</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -3327,7 +3333,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>185</v>
       </c>
@@ -3345,7 +3351,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>188</v>
       </c>
@@ -3354,7 +3360,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>190</v>
       </c>
@@ -3363,7 +3369,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>192</v>
       </c>
@@ -3372,7 +3378,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>194</v>
       </c>
@@ -3393,7 +3399,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>197</v>
       </c>
@@ -3408,7 +3414,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>199</v>
       </c>
@@ -3426,7 +3432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>201</v>
       </c>
@@ -3441,7 +3447,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>203</v>
       </c>
@@ -3453,7 +3459,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>205</v>
       </c>
@@ -3471,7 +3477,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>207</v>
       </c>
@@ -3483,7 +3489,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>209</v>
       </c>
@@ -3498,7 +3504,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>211</v>
       </c>
@@ -3516,7 +3522,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>213</v>
       </c>
@@ -3531,13 +3537,13 @@
         <v>113</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>215</v>
       </c>
       <c r="B79" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>IRI_VALUE_DATE,HPMS_SAMPLE_NO</v>
+        <v>IRI_VALUE_DATE,HPMS_SAMPLE_NO,BEGIN_DATE,F_SYSTEM,NHS,IRI_VALUE_TEXT</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>380</v>
@@ -3545,14 +3551,26 @@
       <c r="D79" s="5" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E79" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>217</v>
       </c>
       <c r="B80" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>RUTTING_VALUE_DATE,HPMS_SAMPLE_NO</v>
+        <v>RUTTING_VALUE_DATE,HPMS_SAMPLE_NO,BEGIN_DATE,F_SYSTEM,NHS,RUTTING_VALUE_TEXT</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>386</v>
@@ -3560,14 +3578,26 @@
       <c r="D80" s="5" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E80" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>218</v>
       </c>
       <c r="B81" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>FAULTING_VALUE_DATE,HPMS_SAMPLE_NO</v>
+        <v>FAULTING_VALUE_DATE,HPMS_SAMPLE_NO,BEGIN_DATE</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>384</v>
@@ -3575,14 +3605,17 @@
       <c r="D81" s="5" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E81" s="5" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>219</v>
       </c>
       <c r="B82" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>CRACKING_PERCENT_VALUE_DATE,HPMS_SAMPLE_NO</v>
+        <v>CRACKING_PERCENT_VALUE_DATE,HPMS_SAMPLE_NO,BEGIN_DATE,F_SYSTEM,NHS,CRACKING_PERCENT_VALUE_TEXT</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>382</v>
@@ -3590,14 +3623,26 @@
       <c r="D82" s="5" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E82" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>221</v>
       </c>
       <c r="B83" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>CRACKING_PERCENT_VALUE_DATE,CRACKING_PERCENT_VALUE_TEXT,F_SYSTEM</v>
+        <v>CRACKING_PERCENT_VALUE_DATE,CRACKING_PERCENT_VALUE_TEXT,F_SYSTEM,BEGIN_DATE</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>382</v>
@@ -3608,14 +3653,17 @@
       <c r="E83" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F83" s="5" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>224</v>
       </c>
       <c r="B84" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>FAULTING_VALUE_DATE,FAULTING_VALUE_TEXT,F_SYSTEM</v>
+        <v>FAULTING_VALUE_DATE,FAULTING_VALUE_TEXT,F_SYSTEM,BEGIN_DATE</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>384</v>
@@ -3626,14 +3674,17 @@
       <c r="E84" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="5" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>226</v>
       </c>
       <c r="B85" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>IRI_VALUE_DATE,IRI_VALUE_TEXT,F_SYSTEM</v>
+        <v>IRI_VALUE_DATE,IRI_VALUE_TEXT,F_SYSTEM,BEGIN_DATE</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>380</v>
@@ -3644,14 +3695,17 @@
       <c r="E85" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="5" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>227</v>
       </c>
       <c r="B86" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>RUTTING_VALUE_DATE,RUTTING_VALUE_TEXT,F_SYSTEM</v>
+        <v>RUTTING_VALUE_DATE,RUTTING_VALUE_TEXT,F_SYSTEM,BEGIN_DATE</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>386</v>
@@ -3662,8 +3716,11 @@
       <c r="E86" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="5" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>229</v>
       </c>
@@ -3684,7 +3741,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>231</v>
       </c>
@@ -3705,7 +3762,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>232</v>
       </c>
@@ -3726,7 +3783,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>233</v>
       </c>
@@ -3747,7 +3804,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>234</v>
       </c>
@@ -3756,7 +3813,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>236</v>
       </c>
@@ -3765,7 +3822,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>238</v>
       </c>
@@ -3774,7 +3831,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>241</v>
       </c>
@@ -3786,7 +3843,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>243</v>
       </c>
@@ -3798,7 +3855,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>245</v>
       </c>
@@ -3813,7 +3870,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="97" spans="1:193" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>247</v>
       </c>
@@ -3828,19 +3885,22 @@
         <v>157</v>
       </c>
     </row>
-    <row r="98" spans="1:193" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>249</v>
       </c>
       <c r="B98" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>YEAR_LAST_CONSTRUCTION_VALUE_DATE</v>
+        <v>YEAR_LAST_CONSTRUCTION_VALUE_DATE,BEGIN_DATE</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="99" spans="1:193" x14ac:dyDescent="0.25">
+      <c r="D98" s="5" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="99" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>251</v>
       </c>
@@ -3855,7 +3915,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="100" spans="1:193" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>254</v>
       </c>
@@ -3870,7 +3930,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="101" spans="1:193" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>256</v>
       </c>
@@ -3885,7 +3945,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="102" spans="1:193" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>258</v>
       </c>
@@ -3900,7 +3960,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="103" spans="1:193" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>260</v>
       </c>
@@ -3915,7 +3975,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="1:193" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>262</v>
       </c>
@@ -3924,7 +3984,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:193" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>265</v>
       </c>
@@ -3939,13 +3999,13 @@
         <v>193</v>
       </c>
     </row>
-    <row r="106" spans="1:193" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>267</v>
       </c>
       <c r="B106" s="6"/>
     </row>
-    <row r="107" spans="1:193" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>270</v>
       </c>
@@ -3966,12 +4026,12 @@
         <v>278</v>
       </c>
     </row>
-    <row r="110" spans="1:193" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="111" spans="1:193" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:194" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>47</v>
       </c>
@@ -4550,6 +4610,9 @@
       </c>
       <c r="GK111" t="s">
         <v>523</v>
+      </c>
+      <c r="GL111" t="s">
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -4569,7 +4632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEACE931-9432-4CAA-874D-46D06D5BC6FB}">
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView topLeftCell="B91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>